<commit_message>
顺序修改 Signed-off-by: LKDE959599 <jiangyanxiong@outlook.com>
</commit_message>
<xml_diff>
--- a/assets/课件/试听课/海洋大冒险/scene/课件编号.xlsx
+++ b/assets/课件/试听课/海洋大冒险/scene/课件编号.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6FACFA-752A-4F9F-B1A5-44A03BBD9CC8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7056E76-9958-486D-9825-687E42BA10A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1410" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>低龄：</t>
   </si>
@@ -473,17 +473,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -499,7 +500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -507,7 +508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -515,7 +516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -523,7 +524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -531,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -539,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -547,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -555,7 +556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -563,7 +564,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -571,7 +572,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -579,7 +580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -587,7 +588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -595,23 +596,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -619,71 +620,68 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
课件上线测试前较大改动 Signed-off-by: LKDE959599 <jiangyanxiong@outlook.com>
</commit_message>
<xml_diff>
--- a/assets/课件/试听课/海洋大冒险/scene/课件编号.xlsx
+++ b/assets/课件/试听课/海洋大冒险/scene/课件编号.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A44C647-F7E4-410D-91A3-B88B14D8D076}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C94812C-6DA9-42E4-B0E8-D6A46A647179}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1410" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11685" yWindow="525" windowWidth="21600" windowHeight="15075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="40">
   <si>
     <t>低龄：</t>
   </si>
@@ -49,91 +49,114 @@
     <t>page9</t>
   </si>
   <si>
+    <t>page13</t>
+  </si>
+  <si>
+    <t>page14</t>
+  </si>
+  <si>
+    <t>page15</t>
+  </si>
+  <si>
+    <t>page16</t>
+  </si>
+  <si>
+    <t>page17</t>
+  </si>
+  <si>
+    <t>page18</t>
+  </si>
+  <si>
+    <t>page19</t>
+  </si>
+  <si>
+    <t>page20</t>
+  </si>
+  <si>
+    <t>page21</t>
+  </si>
+  <si>
+    <t>page22</t>
+  </si>
+  <si>
+    <t>page23</t>
+  </si>
+  <si>
+    <t>page24</t>
+  </si>
+  <si>
+    <t>高龄：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page25</t>
+  </si>
+  <si>
+    <t>page18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低龄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高龄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>page10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>page11</t>
-  </si>
-  <si>
-    <t>page12</t>
-  </si>
-  <si>
-    <t>page13</t>
-  </si>
-  <si>
-    <t>page14</t>
-  </si>
-  <si>
-    <t>page15</t>
-  </si>
-  <si>
-    <t>page16</t>
-  </si>
-  <si>
-    <t>page17</t>
-  </si>
-  <si>
-    <t>page18</t>
-  </si>
-  <si>
-    <t>page19</t>
-  </si>
-  <si>
-    <t>page20</t>
-  </si>
-  <si>
-    <t>page21</t>
-  </si>
-  <si>
-    <t>page22</t>
-  </si>
-  <si>
-    <t>page23</t>
-  </si>
-  <si>
-    <t>page24</t>
-  </si>
-  <si>
-    <t>高龄：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page33</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page34</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page25</t>
-  </si>
-  <si>
-    <t>page18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>page35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page26</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -198,11 +221,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -483,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -496,23 +520,23 @@
     <col min="3" max="3" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -520,185 +544,200 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>31</v>
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
内容修改 Signed-off-by: LKDE959599 <jiangyanxiong@outlook.com>
</commit_message>
<xml_diff>
--- a/assets/课件/试听课/海洋大冒险/scene/课件编号.xlsx
+++ b/assets/课件/试听课/海洋大冒险/scene/课件编号.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F630D6-FE53-442B-94CB-0775BF1FF0A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF4CE9D-1CF8-465E-A832-D5C24DD0BD3C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="1560" windowWidth="21600" windowHeight="15075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="41">
   <si>
     <t>低龄：</t>
   </si>
@@ -199,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +209,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,12 +237,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -511,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -615,9 +629,6 @@
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -632,29 +643,30 @@
         <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
-        <v>30</v>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -679,71 +691,79 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
       <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" s="5" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
课件修改 Signed-off-by: LKDE959599 <jiangyanxiong@outlook.com>
</commit_message>
<xml_diff>
--- a/assets/课件/试听课/海洋大冒险/scene/课件编号.xlsx
+++ b/assets/课件/试听课/海洋大冒险/scene/课件编号.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF4CE9D-1CF8-465E-A832-D5C24DD0BD3C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4041C6-6AF8-4381-AA2D-77D2D2AC651B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>低龄：</t>
   </si>
@@ -161,6 +161,50 @@
   </si>
   <si>
     <t>无12页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低龄：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page55</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -525,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I20" sqref="I2:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -538,31 +582,49 @@
     <col min="3" max="3" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -575,8 +637,14 @@
       <c r="F4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -589,72 +657,123 @@
       <c r="F5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -662,48 +781,87 @@
       <c r="E14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -711,7 +869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -719,7 +877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -727,7 +885,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>17</v>
       </c>
@@ -735,7 +893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -743,7 +901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -751,7 +909,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
@@ -759,7 +917,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>

</xml_diff>